<commit_message>
Fixed Import users and absence of settings
</commit_message>
<xml_diff>
--- a/public/users.xlsx
+++ b/public/users.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>username</t>
   </si>
@@ -38,49 +38,49 @@
     <t>last_name</t>
   </si>
   <si>
-    <t>type</t>
-  </si>
-  <si>
     <t>enrollment_id</t>
   </si>
   <si>
-    <t>class_id</t>
-  </si>
-  <si>
     <t>Daniel</t>
   </si>
   <si>
-    <t>d@d.dd</t>
-  </si>
-  <si>
-    <t>De</t>
-  </si>
-  <si>
-    <t>Sam</t>
-  </si>
-  <si>
-    <t>s@s.ss</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
     <t>password_confirmation</t>
   </si>
   <si>
-    <t>Manajit</t>
-  </si>
-  <si>
-    <t>m@m.mm</t>
-  </si>
-  <si>
-    <t>Manajitt</t>
-  </si>
-  <si>
-    <t>R</t>
+    <t>jsmith</t>
+  </si>
+  <si>
+    <t>rwilliams</t>
+  </si>
+  <si>
+    <t>dhathaway</t>
+  </si>
+  <si>
+    <t>rwilliams@geronimo.com</t>
+  </si>
+  <si>
+    <t>Rory</t>
+  </si>
+  <si>
+    <t>Williams</t>
+  </si>
+  <si>
+    <t>jsmith@geronimo.com</t>
+  </si>
+  <si>
+    <t>Jane</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>dhathaway@geronimo.com</t>
+  </si>
+  <si>
+    <t>Hathaway</t>
   </si>
 </sst>
 </file>
@@ -409,15 +409,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="12.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -434,104 +437,84 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2">
+        <v>1234</v>
+      </c>
+      <c r="G2">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3">
+        <v>1020</v>
+      </c>
+      <c r="F3">
+        <v>1234</v>
+      </c>
+      <c r="G3">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>1234</v>
-      </c>
-      <c r="I2">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-      <c r="F3">
-        <v>1020</v>
-      </c>
-      <c r="G3">
-        <v>2</v>
-      </c>
-      <c r="H3">
-        <v>1234</v>
-      </c>
-      <c r="I3">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
       </c>
       <c r="D4" t="s">
         <v>18</v>
       </c>
       <c r="E4">
-        <v>3</v>
+        <v>1021</v>
       </c>
       <c r="F4">
-        <v>1021</v>
+        <v>1234</v>
       </c>
       <c r="G4">
-        <v>2</v>
-      </c>
-      <c r="H4">
-        <v>1234</v>
-      </c>
-      <c r="I4">
         <v>1234</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B3:B4" r:id="rId2" display="rwilliams@geronimo.com"/>
+    <hyperlink ref="B3" r:id="rId3"/>
+    <hyperlink ref="B4" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert "Revert "UI changes""
This reverts commit 672c653c2deaa5293e19f1e48284efde9db4a34e.
</commit_message>
<xml_diff>
--- a/public/users.xlsx
+++ b/public/users.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmiyan\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20910"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9360"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -24,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>username</t>
   </si>
@@ -42,12 +40,6 @@
   </si>
   <si>
     <t>Daniel</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>password_confirmation</t>
   </si>
   <si>
     <t>jsmith</t>
@@ -189,7 +181,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -224,7 +216,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -401,7 +393,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -409,18 +401,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="5" max="5" width="12.5546875" customWidth="1"/>
+    <col min="5" max="5" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -436,77 +428,56 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="F2">
-        <v>1234</v>
-      </c>
-      <c r="G2">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" t="s">
         <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
       </c>
       <c r="E3">
         <v>1020</v>
       </c>
-      <c r="F3">
-        <v>1234</v>
-      </c>
-      <c r="G3">
-        <v>1234</v>
-      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E4">
         <v>1021</v>
-      </c>
-      <c r="F4">
-        <v>1234</v>
-      </c>
-      <c r="G4">
-        <v>1234</v>
       </c>
     </row>
   </sheetData>
@@ -517,5 +488,10 @@
     <hyperlink ref="B4" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>